<commit_message>
Rubric, and final clean up
</commit_message>
<xml_diff>
--- a/Tekle_Amanuel_capstone2_rubric.xlsx
+++ b/Tekle_Amanuel_capstone2_rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanu\Documents\DB Bootcamp Cohort 3\Capstone2\Tekle_Amanuel_Capstone2\Tek-Tekle-Capstone2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5ED59B21-F46F-4DC7-9585-9FD61E771952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4D0351-D41B-4D54-BD7B-727C26C82323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05EE201A-0BCA-5646-B296-5AABFBEA194B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{05EE201A-0BCA-5646-B296-5AABFBEA194B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cap2 Rubric Pt 1" sheetId="99" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="129">
   <si>
     <t>Functionality</t>
   </si>
@@ -405,6 +405,27 @@
   </si>
   <si>
     <t xml:space="preserve">What tutorials, if any, did you leverage most in building this project? This question is important for assessing integrity. </t>
+  </si>
+  <si>
+    <t>Amanuel Tekle</t>
+  </si>
+  <si>
+    <t>https://github.com/Amanuel2022/Tek-Tekle-Capstone2.git</t>
+  </si>
+  <si>
+    <t>To come up with a solution for this expercise I had to use all my resources. I went back and watched some lectures, watched a lot of youtube videos, the Udemy and looked back on my past work.</t>
+  </si>
+  <si>
+    <t>To run this program you can simply look through the different sections and filter the data for year, team and player. You also have the option to drill through. To use the you need to right click and press drill through to the page you want to see next. I also set up a few buttons go back one page, go home, and clear filter.</t>
+  </si>
+  <si>
+    <t>Challenges I ran into during this exercise is, finding the right data set. Even when you think you found a good dataset, checking the accuracy, the nulls and trying to plan ahead for different types of visulization and story.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The most imporant thing I learned during this exercise would have to be given more time and more experience how fun exploring data could be. Trying to find something that hasn’t been found or even trying to prove/disprove an idea you had about the data/subject. </t>
+  </si>
+  <si>
+    <t>For the project I leveraged a lot of youtube videos of a few things here and a few things there but did not follow any kind of tutorial or step by step to build my project. I tried to use all my resources.</t>
   </si>
 </sst>
 </file>
@@ -1610,8 +1631,8 @@
   </sheetPr>
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1646,7 +1667,9 @@
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="30"/>
+      <c r="B2" s="30" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="3" spans="1:23" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="8"/>
@@ -2366,8 +2389,8 @@
   </sheetPr>
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2393,7 +2416,9 @@
       <c r="B5" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="6" spans="2:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
@@ -2405,31 +2430,41 @@
       <c r="B7" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="8" spans="2:3" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="2:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C8" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="2:3" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C9" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="11" spans="2:3" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2441,12 +2476,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d2a9f884-c2eb-4182-8d97-b2c1069a1e77">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="872877ae-a410-445f-835b-653367d2e530" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2686,20 +2723,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d2a9f884-c2eb-4182-8d97-b2c1069a1e77">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="872877ae-a410-445f-835b-653367d2e530" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8A09A7-4930-415E-BC0E-99BBC8E2BDB5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DCCBC0B-BA77-41C1-B14F-94133CE8E251}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="ad1dcd44-2c79-421e-996d-e07b6b6a06b7"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d2a9f884-c2eb-4182-8d97-b2c1069a1e77"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="872877ae-a410-445f-835b-653367d2e530"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2725,19 +2770,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DCCBC0B-BA77-41C1-B14F-94133CE8E251}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8A09A7-4930-415E-BC0E-99BBC8E2BDB5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="ad1dcd44-2c79-421e-996d-e07b6b6a06b7"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d2a9f884-c2eb-4182-8d97-b2c1069a1e77"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="872877ae-a410-445f-835b-653367d2e530"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Last minute clean up
</commit_message>
<xml_diff>
--- a/Tekle_Amanuel_capstone2_rubric.xlsx
+++ b/Tekle_Amanuel_capstone2_rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amanu\Documents\DB Bootcamp Cohort 3\Capstone2\Tekle_Amanuel_Capstone2\Tek-Tekle-Capstone2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4D0351-D41B-4D54-BD7B-727C26C82323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6247DFA8-50E1-4E82-9139-B3E95BCAE6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{05EE201A-0BCA-5646-B296-5AABFBEA194B}"/>
+    <workbookView xWindow="5796" yWindow="792" windowWidth="17232" windowHeight="11088" firstSheet="1" activeTab="1" xr2:uid="{05EE201A-0BCA-5646-B296-5AABFBEA194B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cap2 Rubric Pt 1" sheetId="99" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
   <si>
     <t>Functionality</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>For the project I leveraged a lot of youtube videos of a few things here and a few things there but did not follow any kind of tutorial or step by step to build my project. I tried to use all my resources.</t>
+  </si>
+  <si>
+    <t>Tekle_Amanuel_Capstone2.zip</t>
   </si>
 </sst>
 </file>
@@ -2389,8 +2392,8 @@
   </sheetPr>
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2424,7 +2427,9 @@
       <c r="B6" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="7" spans="2:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
@@ -2487,6 +2492,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FEF7458C51E57141848015B90E19E3FF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12fb0db276e8be4984a0823ffe929ad1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d2a9f884-c2eb-4182-8d97-b2c1069a1e77" xmlns:ns3="ad1dcd44-2c79-421e-996d-e07b6b6a06b7" xmlns:ns4="872877ae-a410-445f-835b-653367d2e530" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f400bb4bb80b6365717ab8834d3c4dc" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="d2a9f884-c2eb-4182-8d97-b2c1069a1e77"/>
@@ -2722,15 +2736,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DCCBC0B-BA77-41C1-B14F-94133CE8E251}">
   <ds:schemaRefs>
@@ -2750,6 +2755,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8A09A7-4930-415E-BC0E-99BBC8E2BDB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E756C58-C06E-42EA-8B82-C61BBA13C316}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2767,12 +2780,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8A09A7-4930-415E-BC0E-99BBC8E2BDB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>